<commit_message>
After completing email functionality
</commit_message>
<xml_diff>
--- a/SandlerTrainingSLN/Documents/Aug-Sept/CompanyLoadTest.xlsx
+++ b/SandlerTrainingSLN/Documents/Aug-Sept/CompanyLoadTest.xlsx
@@ -105,9 +105,6 @@
     <t>Hamish</t>
   </si>
   <si>
-    <t>ABL Imaging Group Inc.</t>
-  </si>
-  <si>
     <t>T2G 0X8</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>230 11th Avenue SE</t>
+  </si>
+  <si>
+    <t>XYZ Test Inc</t>
   </si>
 </sst>
 </file>
@@ -178,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -201,6 +201,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,7 +507,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,8 +593,8 @@
       <c r="A2" s="6">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>29</v>
+      <c r="B2" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>25</v>
@@ -602,16 +603,16 @@
         <v>26</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="I2" s="7">
         <v>0</v>
@@ -642,7 +643,7 @@
       <c r="U2" s="10"/>
       <c r="V2" s="3"/>
       <c r="Y2" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>